<commit_message>
PDF za 02 dodan
</commit_message>
<xml_diff>
--- a/02_Delo_s_podatki/viri/primer2.xlsx
+++ b/02_Delo_s_podatki/viri/primer2.xlsx
@@ -1,76 +1,82 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13120" windowHeight="6100"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t xml:space="preserve">Ime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priimek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">st_prijateljev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Št_prijateljev_na_leto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arčon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kovač</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Janko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zelenko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pečar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Črt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Žerjal</t>
+    <t>Ime</t>
+  </si>
+  <si>
+    <t>Priimek</t>
+  </si>
+  <si>
+    <t>Starost</t>
+  </si>
+  <si>
+    <t>st_prijateljev</t>
+  </si>
+  <si>
+    <t>Janez</t>
+  </si>
+  <si>
+    <t>Novak</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Arčon</t>
+  </si>
+  <si>
+    <t>Miha</t>
+  </si>
+  <si>
+    <t>Kovač</t>
+  </si>
+  <si>
+    <t>Janko</t>
+  </si>
+  <si>
+    <t>Zelenko</t>
+  </si>
+  <si>
+    <t>Metka</t>
+  </si>
+  <si>
+    <t>Pečar</t>
+  </si>
+  <si>
+    <t>Črt</t>
+  </si>
+  <si>
+    <t>Žerjal</t>
+  </si>
+  <si>
+    <t>Št_prij_leto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,6 +112,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -387,14 +394,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,113 +417,118 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="n">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>66</v>
+      </c>
+      <c r="E3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="n">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
         <v>23</v>
       </c>
-      <c r="E2" t="n">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>66</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="n">
-        <v>13</v>
-      </c>
-      <c r="D4" t="n">
-        <v>40</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3.08</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="n">
-        <v>22</v>
-      </c>
-      <c r="D5" t="n">
-        <v>27</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D6">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="n">
-        <v>23</v>
-      </c>
-      <c r="D6" t="n">
-        <v>33</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>34</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>193</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>5.68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>